<commit_message>
Edited some of the dl docs
Had to take out some additioanl things from the documents you can download to remove any confidential information.
</commit_message>
<xml_diff>
--- a/cost_optimization_for_installation_operations/excel/cost_optimization_for_installation_operations.xlsx
+++ b/cost_optimization_for_installation_operations/excel/cost_optimization_for_installation_operations.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\OneDrive\Desktop\Resume and Career\Github\Cost Optimizations for Installation Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08716ED-18DE-43AD-AE96-23BCDAD746DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B153FCA-0D6C-4E1E-A973-290680CA9BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Info For PowerPoint" sheetId="16" r:id="rId1"/>
-    <sheet name="Projected Savings" sheetId="11" r:id="rId2"/>
+    <sheet name="Projected Savings" sheetId="11" r:id="rId1"/>
+    <sheet name="Info For PowerPoint" sheetId="16" r:id="rId2"/>
     <sheet name="3rd Party 2 Install Data" sheetId="17" r:id="rId3"/>
     <sheet name="3rd Party 1 Install Data" sheetId="15" r:id="rId4"/>
     <sheet name="Maine Region Data" sheetId="3" r:id="rId5"/>
-    <sheet name="Maine Heat Map" sheetId="7" r:id="rId6"/>
-    <sheet name="Maine Region Map" sheetId="8" r:id="rId7"/>
+    <sheet name="Maine Heat Map" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="Maine Region Map" sheetId="8" state="hidden" r:id="rId7"/>
     <sheet name="Zip Code Regions" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1405,6 +1405,972 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE11675F-C71B-4A48-88CE-FC87F2DC1B89}">
+  <dimension ref="A1:R67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="62" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="62" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A44" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="82"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="82"/>
+      <c r="H44" s="82"/>
+      <c r="J44" s="82" t="s">
+        <v>93</v>
+      </c>
+      <c r="K44" s="82"/>
+      <c r="L44" s="82"/>
+      <c r="M44" s="82"/>
+      <c r="N44" s="82"/>
+      <c r="O44" s="82"/>
+      <c r="P44" s="82"/>
+      <c r="Q44" s="82"/>
+    </row>
+    <row r="45" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="K45" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="M45" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="N45" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="O45" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="P45" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q45" s="45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="35">
+        <v>53950</v>
+      </c>
+      <c r="C46" s="7">
+        <v>17905.999999999971</v>
+      </c>
+      <c r="D46" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E46" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F46" s="7">
+        <v>22080</v>
+      </c>
+      <c r="G46" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H46" s="31">
+        <v>200</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="35">
+        <v>85583</v>
+      </c>
+      <c r="L46" s="7">
+        <v>39430.999999999942</v>
+      </c>
+      <c r="M46" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N46" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O46" s="7">
+        <v>25820</v>
+      </c>
+      <c r="P46" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q46" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="35">
+        <v>69582.5</v>
+      </c>
+      <c r="C47" s="7">
+        <v>11954.999999999971</v>
+      </c>
+      <c r="D47" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E47" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F47" s="7">
+        <v>31760</v>
+      </c>
+      <c r="G47" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H47" s="31">
+        <v>200</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K47" s="35">
+        <v>70717.5</v>
+      </c>
+      <c r="L47" s="7">
+        <v>21988.999999999971</v>
+      </c>
+      <c r="M47" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N47" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O47" s="7">
+        <v>36600</v>
+      </c>
+      <c r="P47" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q47" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="35">
+        <v>83273.5</v>
+      </c>
+      <c r="C48" s="7">
+        <v>37749.999999999942</v>
+      </c>
+      <c r="D48" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E48" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F48" s="7">
+        <v>33520</v>
+      </c>
+      <c r="G48" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H48" s="31">
+        <v>200</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" s="35">
+        <v>112905.5</v>
+      </c>
+      <c r="L48" s="7">
+        <v>51285.999999999942</v>
+      </c>
+      <c r="M48" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N48" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O48" s="7">
+        <v>72020</v>
+      </c>
+      <c r="P48" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q48" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="35">
+        <v>30491.5</v>
+      </c>
+      <c r="C49" s="7">
+        <v>13638.999999999985</v>
+      </c>
+      <c r="D49" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E49" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F49" s="7">
+        <v>12180</v>
+      </c>
+      <c r="G49" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H49" s="31">
+        <v>200</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="35">
+        <v>38426.5</v>
+      </c>
+      <c r="L49" s="7">
+        <v>15525.999999999985</v>
+      </c>
+      <c r="M49" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N49" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O49" s="7">
+        <v>19880</v>
+      </c>
+      <c r="P49" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q49" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="35">
+        <v>5970</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1577.9999999999964</v>
+      </c>
+      <c r="D50" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E50" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F50" s="7">
+        <v>2500</v>
+      </c>
+      <c r="G50" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H50" s="31">
+        <v>200</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="35">
+        <v>5042.5</v>
+      </c>
+      <c r="L50" s="7">
+        <v>1474.9999999999982</v>
+      </c>
+      <c r="M50" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N50" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O50" s="7">
+        <v>3600</v>
+      </c>
+      <c r="P50" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q50" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="41">
+        <v>21220.5</v>
+      </c>
+      <c r="C51" s="7">
+        <v>6642.9999999999927</v>
+      </c>
+      <c r="D51" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="E51" s="31">
+        <v>15000</v>
+      </c>
+      <c r="F51" s="7">
+        <v>7340</v>
+      </c>
+      <c r="G51" s="7">
+        <v>20000</v>
+      </c>
+      <c r="H51" s="31">
+        <v>200</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K51" s="41">
+        <v>32612</v>
+      </c>
+      <c r="L51" s="7">
+        <v>13112.999999999985</v>
+      </c>
+      <c r="M51" s="49">
+        <v>38722.666666666672</v>
+      </c>
+      <c r="N51" s="31">
+        <v>15000</v>
+      </c>
+      <c r="O51" s="7">
+        <v>15040</v>
+      </c>
+      <c r="P51" s="7">
+        <v>20000</v>
+      </c>
+      <c r="Q51" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="22">
+        <v>264488</v>
+      </c>
+      <c r="C52" s="20">
+        <v>89470.999999999854</v>
+      </c>
+      <c r="D52" s="50">
+        <v>232336.00000000006</v>
+      </c>
+      <c r="E52" s="42">
+        <v>90000</v>
+      </c>
+      <c r="F52" s="22">
+        <v>109380</v>
+      </c>
+      <c r="G52" s="22">
+        <v>120000</v>
+      </c>
+      <c r="H52" s="42">
+        <v>1200</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="K52" s="22">
+        <v>345287</v>
+      </c>
+      <c r="L52" s="20">
+        <v>142819.99999999983</v>
+      </c>
+      <c r="M52" s="50">
+        <v>232336.00000000006</v>
+      </c>
+      <c r="N52" s="42">
+        <v>90000</v>
+      </c>
+      <c r="O52" s="22">
+        <v>172960</v>
+      </c>
+      <c r="P52" s="22">
+        <v>120000</v>
+      </c>
+      <c r="Q52" s="42">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="81" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="81"/>
+      <c r="J54" s="81" t="s">
+        <v>78</v>
+      </c>
+      <c r="K54" s="81"/>
+      <c r="L54" s="81"/>
+      <c r="M54" s="81"/>
+      <c r="N54" s="81"/>
+      <c r="O54" s="81"/>
+      <c r="P54" s="81"/>
+      <c r="Q54" s="81"/>
+    </row>
+    <row r="55" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="83">
+        <v>-198957.00000000012</v>
+      </c>
+      <c r="B55" s="83"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="83"/>
+      <c r="J55" s="83">
+        <v>-128389.00000000017</v>
+      </c>
+      <c r="K55" s="83"/>
+      <c r="L55" s="83"/>
+      <c r="M55" s="83"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="83"/>
+      <c r="Q55" s="83"/>
+    </row>
+    <row r="56" spans="1:18" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="81"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
+      <c r="F57" s="81"/>
+      <c r="G57" s="81"/>
+      <c r="H57" s="81"/>
+      <c r="J57" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="K57" s="81"/>
+      <c r="L57" s="81"/>
+      <c r="M57" s="81"/>
+      <c r="N57" s="81"/>
+      <c r="O57" s="81"/>
+      <c r="P57" s="81"/>
+      <c r="Q57" s="81"/>
+    </row>
+    <row r="58" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="84">
+        <v>465000</v>
+      </c>
+      <c r="B58" s="84"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84"/>
+      <c r="G58" s="84"/>
+      <c r="H58" s="84"/>
+      <c r="J58" s="84">
+        <v>465000</v>
+      </c>
+      <c r="K58" s="84"/>
+      <c r="L58" s="84"/>
+      <c r="M58" s="84"/>
+      <c r="N58" s="84"/>
+      <c r="O58" s="84"/>
+      <c r="P58" s="84"/>
+      <c r="Q58" s="84"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="7">
+        <v>6831.586842105261</v>
+      </c>
+      <c r="E59" t="s">
+        <v>118</v>
+      </c>
+      <c r="F59" s="76">
+        <v>7989.6320469798648</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B60" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="7">
+        <v>7625.8285326086952</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="48.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="L61" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="M61" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="P61" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q61" s="74" t="s">
+        <v>91</v>
+      </c>
+      <c r="R61" s="74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" s="4">
+        <v>120960</v>
+      </c>
+      <c r="L62" s="4">
+        <v>79040</v>
+      </c>
+      <c r="M62" s="4">
+        <v>182094.00000000003</v>
+      </c>
+      <c r="O62" t="s">
+        <v>27</v>
+      </c>
+      <c r="P62" s="4">
+        <v>309120</v>
+      </c>
+      <c r="Q62" s="4">
+        <v>15200</v>
+      </c>
+      <c r="R62" s="4">
+        <v>284889.00000000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" s="4">
+        <v>33600</v>
+      </c>
+      <c r="L63" s="4">
+        <v>228000</v>
+      </c>
+      <c r="M63" s="4">
+        <v>249645.00000000003</v>
+      </c>
+      <c r="O63" t="s">
+        <v>26</v>
+      </c>
+      <c r="P63" s="4">
+        <v>141120</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>124640</v>
+      </c>
+      <c r="R63" s="4">
+        <v>243771.00000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>21</v>
+      </c>
+      <c r="K64" s="4">
+        <v>299040</v>
+      </c>
+      <c r="L64" s="4">
+        <v>3040</v>
+      </c>
+      <c r="M64" s="4">
+        <v>264330.00000000006</v>
+      </c>
+      <c r="O64" t="s">
+        <v>21</v>
+      </c>
+      <c r="P64" s="4">
+        <v>406560</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>3040</v>
+      </c>
+      <c r="R64" s="4">
+        <v>358314.00000000006</v>
+      </c>
+    </row>
+    <row r="65" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" s="4">
+        <v>107520</v>
+      </c>
+      <c r="L65" s="4">
+        <v>3040</v>
+      </c>
+      <c r="M65" s="4">
+        <v>96921.000000000015</v>
+      </c>
+      <c r="O65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P65" s="4">
+        <v>117600</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>21280</v>
+      </c>
+      <c r="R65" s="4">
+        <v>123354.00000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>25</v>
+      </c>
+      <c r="K66" s="4">
+        <v>10080</v>
+      </c>
+      <c r="L66" s="4">
+        <v>9120</v>
+      </c>
+      <c r="M66" s="4">
+        <v>17622.000000000004</v>
+      </c>
+      <c r="O66" t="s">
+        <v>25</v>
+      </c>
+      <c r="P66" s="4">
+        <v>10080</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>6080</v>
+      </c>
+      <c r="R66" s="4">
+        <v>14685.000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>20</v>
+      </c>
+      <c r="K67" s="4">
+        <v>47040</v>
+      </c>
+      <c r="L67" s="4">
+        <v>21280</v>
+      </c>
+      <c r="M67" s="4">
+        <v>61677.000000000007</v>
+      </c>
+      <c r="O67" t="s">
+        <v>20</v>
+      </c>
+      <c r="P67" s="4">
+        <v>104160</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>0</v>
+      </c>
+      <c r="R67" s="4">
+        <v>91047.000000000015</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A58:H58"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="J44:Q44"/>
+    <mergeCell ref="J54:Q54"/>
+    <mergeCell ref="J55:Q55"/>
+    <mergeCell ref="J57:Q57"/>
+    <mergeCell ref="J58:Q58"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3430E7-5C78-4FBD-8CF9-B3DA47BC521D}">
   <dimension ref="A1:AD27"/>
   <sheetViews>
@@ -2887,972 +3853,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE11675F-C71B-4A48-88CE-FC87F2DC1B89}">
-  <dimension ref="A1:R67"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44:Q44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="62" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="82" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="82"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="J44" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="K44" s="82"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="82"/>
-      <c r="O44" s="82"/>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="82"/>
-    </row>
-    <row r="45" spans="1:17" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="F45" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="H45" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="I45" s="2"/>
-      <c r="K45" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="L45" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="M45" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="N45" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="O45" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="P45" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q45" s="45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="35">
-        <v>53950</v>
-      </c>
-      <c r="C46" s="7">
-        <v>17905.999999999971</v>
-      </c>
-      <c r="D46" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E46" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F46" s="7">
-        <v>22080</v>
-      </c>
-      <c r="G46" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H46" s="31">
-        <v>200</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K46" s="35">
-        <v>85583</v>
-      </c>
-      <c r="L46" s="7">
-        <v>39430.999999999942</v>
-      </c>
-      <c r="M46" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N46" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O46" s="7">
-        <v>25820</v>
-      </c>
-      <c r="P46" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q46" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="35">
-        <v>69582.5</v>
-      </c>
-      <c r="C47" s="7">
-        <v>11954.999999999971</v>
-      </c>
-      <c r="D47" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E47" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F47" s="7">
-        <v>31760</v>
-      </c>
-      <c r="G47" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H47" s="31">
-        <v>200</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K47" s="35">
-        <v>70717.5</v>
-      </c>
-      <c r="L47" s="7">
-        <v>21988.999999999971</v>
-      </c>
-      <c r="M47" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N47" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O47" s="7">
-        <v>36600</v>
-      </c>
-      <c r="P47" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q47" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="35">
-        <v>83273.5</v>
-      </c>
-      <c r="C48" s="7">
-        <v>37749.999999999942</v>
-      </c>
-      <c r="D48" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E48" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F48" s="7">
-        <v>33520</v>
-      </c>
-      <c r="G48" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H48" s="31">
-        <v>200</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K48" s="35">
-        <v>112905.5</v>
-      </c>
-      <c r="L48" s="7">
-        <v>51285.999999999942</v>
-      </c>
-      <c r="M48" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N48" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O48" s="7">
-        <v>72020</v>
-      </c>
-      <c r="P48" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q48" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B49" s="35">
-        <v>30491.5</v>
-      </c>
-      <c r="C49" s="7">
-        <v>13638.999999999985</v>
-      </c>
-      <c r="D49" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E49" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F49" s="7">
-        <v>12180</v>
-      </c>
-      <c r="G49" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H49" s="31">
-        <v>200</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K49" s="35">
-        <v>38426.5</v>
-      </c>
-      <c r="L49" s="7">
-        <v>15525.999999999985</v>
-      </c>
-      <c r="M49" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N49" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O49" s="7">
-        <v>19880</v>
-      </c>
-      <c r="P49" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q49" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="35">
-        <v>5970</v>
-      </c>
-      <c r="C50" s="7">
-        <v>1577.9999999999964</v>
-      </c>
-      <c r="D50" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E50" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F50" s="7">
-        <v>2500</v>
-      </c>
-      <c r="G50" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H50" s="31">
-        <v>200</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="35">
-        <v>5042.5</v>
-      </c>
-      <c r="L50" s="7">
-        <v>1474.9999999999982</v>
-      </c>
-      <c r="M50" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N50" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O50" s="7">
-        <v>3600</v>
-      </c>
-      <c r="P50" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q50" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="41">
-        <v>21220.5</v>
-      </c>
-      <c r="C51" s="7">
-        <v>6642.9999999999927</v>
-      </c>
-      <c r="D51" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="E51" s="31">
-        <v>15000</v>
-      </c>
-      <c r="F51" s="7">
-        <v>7340</v>
-      </c>
-      <c r="G51" s="7">
-        <v>20000</v>
-      </c>
-      <c r="H51" s="31">
-        <v>200</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" s="41">
-        <v>32612</v>
-      </c>
-      <c r="L51" s="7">
-        <v>13112.999999999985</v>
-      </c>
-      <c r="M51" s="49">
-        <v>38722.666666666672</v>
-      </c>
-      <c r="N51" s="31">
-        <v>15000</v>
-      </c>
-      <c r="O51" s="7">
-        <v>15040</v>
-      </c>
-      <c r="P51" s="7">
-        <v>20000</v>
-      </c>
-      <c r="Q51" s="31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="22">
-        <v>264488</v>
-      </c>
-      <c r="C52" s="20">
-        <v>89470.999999999854</v>
-      </c>
-      <c r="D52" s="50">
-        <v>232336.00000000006</v>
-      </c>
-      <c r="E52" s="42">
-        <v>90000</v>
-      </c>
-      <c r="F52" s="22">
-        <v>109380</v>
-      </c>
-      <c r="G52" s="22">
-        <v>120000</v>
-      </c>
-      <c r="H52" s="42">
-        <v>1200</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="K52" s="22">
-        <v>345287</v>
-      </c>
-      <c r="L52" s="20">
-        <v>142819.99999999983</v>
-      </c>
-      <c r="M52" s="50">
-        <v>232336.00000000006</v>
-      </c>
-      <c r="N52" s="42">
-        <v>90000</v>
-      </c>
-      <c r="O52" s="22">
-        <v>172960</v>
-      </c>
-      <c r="P52" s="22">
-        <v>120000</v>
-      </c>
-      <c r="Q52" s="42">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="81"/>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
-      <c r="G54" s="81"/>
-      <c r="H54" s="81"/>
-      <c r="J54" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="K54" s="81"/>
-      <c r="L54" s="81"/>
-      <c r="M54" s="81"/>
-      <c r="N54" s="81"/>
-      <c r="O54" s="81"/>
-      <c r="P54" s="81"/>
-      <c r="Q54" s="81"/>
-    </row>
-    <row r="55" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="83">
-        <v>-198957.00000000012</v>
-      </c>
-      <c r="B55" s="83"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="83"/>
-      <c r="E55" s="83"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="J55" s="83">
-        <v>-128389.00000000017</v>
-      </c>
-      <c r="K55" s="83"/>
-      <c r="L55" s="83"/>
-      <c r="M55" s="83"/>
-      <c r="N55" s="83"/>
-      <c r="O55" s="83"/>
-      <c r="P55" s="83"/>
-      <c r="Q55" s="83"/>
-    </row>
-    <row r="56" spans="1:18" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="81"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
-      <c r="F57" s="81"/>
-      <c r="G57" s="81"/>
-      <c r="H57" s="81"/>
-      <c r="J57" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="K57" s="81"/>
-      <c r="L57" s="81"/>
-      <c r="M57" s="81"/>
-      <c r="N57" s="81"/>
-      <c r="O57" s="81"/>
-      <c r="P57" s="81"/>
-      <c r="Q57" s="81"/>
-    </row>
-    <row r="58" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="84">
-        <v>465000</v>
-      </c>
-      <c r="B58" s="84"/>
-      <c r="C58" s="84"/>
-      <c r="D58" s="84"/>
-      <c r="E58" s="84"/>
-      <c r="F58" s="84"/>
-      <c r="G58" s="84"/>
-      <c r="H58" s="84"/>
-      <c r="J58" s="84">
-        <v>465000</v>
-      </c>
-      <c r="K58" s="84"/>
-      <c r="L58" s="84"/>
-      <c r="M58" s="84"/>
-      <c r="N58" s="84"/>
-      <c r="O58" s="84"/>
-      <c r="P58" s="84"/>
-      <c r="Q58" s="84"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="C59" s="7">
-        <v>6831.586842105261</v>
-      </c>
-      <c r="E59" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" s="76">
-        <v>7989.6320469798648</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="7">
-        <v>7625.8285326086952</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="48.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="K61" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="L61" s="74" t="s">
-        <v>91</v>
-      </c>
-      <c r="M61" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="P61" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q61" s="74" t="s">
-        <v>91</v>
-      </c>
-      <c r="R61" s="74" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J62" t="s">
-        <v>27</v>
-      </c>
-      <c r="K62" s="4">
-        <v>120960</v>
-      </c>
-      <c r="L62" s="4">
-        <v>79040</v>
-      </c>
-      <c r="M62" s="4">
-        <v>182094.00000000003</v>
-      </c>
-      <c r="O62" t="s">
-        <v>27</v>
-      </c>
-      <c r="P62" s="4">
-        <v>309120</v>
-      </c>
-      <c r="Q62" s="4">
-        <v>15200</v>
-      </c>
-      <c r="R62" s="4">
-        <v>284889.00000000006</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J63" t="s">
-        <v>26</v>
-      </c>
-      <c r="K63" s="4">
-        <v>33600</v>
-      </c>
-      <c r="L63" s="4">
-        <v>228000</v>
-      </c>
-      <c r="M63" s="4">
-        <v>249645.00000000003</v>
-      </c>
-      <c r="O63" t="s">
-        <v>26</v>
-      </c>
-      <c r="P63" s="4">
-        <v>141120</v>
-      </c>
-      <c r="Q63" s="4">
-        <v>124640</v>
-      </c>
-      <c r="R63" s="4">
-        <v>243771.00000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J64" t="s">
-        <v>21</v>
-      </c>
-      <c r="K64" s="4">
-        <v>299040</v>
-      </c>
-      <c r="L64" s="4">
-        <v>3040</v>
-      </c>
-      <c r="M64" s="4">
-        <v>264330.00000000006</v>
-      </c>
-      <c r="O64" t="s">
-        <v>21</v>
-      </c>
-      <c r="P64" s="4">
-        <v>406560</v>
-      </c>
-      <c r="Q64" s="4">
-        <v>3040</v>
-      </c>
-      <c r="R64" s="4">
-        <v>358314.00000000006</v>
-      </c>
-    </row>
-    <row r="65" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J65" t="s">
-        <v>28</v>
-      </c>
-      <c r="K65" s="4">
-        <v>107520</v>
-      </c>
-      <c r="L65" s="4">
-        <v>3040</v>
-      </c>
-      <c r="M65" s="4">
-        <v>96921.000000000015</v>
-      </c>
-      <c r="O65" t="s">
-        <v>28</v>
-      </c>
-      <c r="P65" s="4">
-        <v>117600</v>
-      </c>
-      <c r="Q65" s="4">
-        <v>21280</v>
-      </c>
-      <c r="R65" s="4">
-        <v>123354.00000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J66" t="s">
-        <v>25</v>
-      </c>
-      <c r="K66" s="4">
-        <v>10080</v>
-      </c>
-      <c r="L66" s="4">
-        <v>9120</v>
-      </c>
-      <c r="M66" s="4">
-        <v>17622.000000000004</v>
-      </c>
-      <c r="O66" t="s">
-        <v>25</v>
-      </c>
-      <c r="P66" s="4">
-        <v>10080</v>
-      </c>
-      <c r="Q66" s="4">
-        <v>6080</v>
-      </c>
-      <c r="R66" s="4">
-        <v>14685.000000000002</v>
-      </c>
-    </row>
-    <row r="67" spans="10:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="J67" t="s">
-        <v>20</v>
-      </c>
-      <c r="K67" s="4">
-        <v>47040</v>
-      </c>
-      <c r="L67" s="4">
-        <v>21280</v>
-      </c>
-      <c r="M67" s="4">
-        <v>61677.000000000007</v>
-      </c>
-      <c r="O67" t="s">
-        <v>20</v>
-      </c>
-      <c r="P67" s="4">
-        <v>104160</v>
-      </c>
-      <c r="Q67" s="4">
-        <v>0</v>
-      </c>
-      <c r="R67" s="4">
-        <v>91047.000000000015</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A58:H58"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="J44:Q44"/>
-    <mergeCell ref="J54:Q54"/>
-    <mergeCell ref="J55:Q55"/>
-    <mergeCell ref="J57:Q57"/>
-    <mergeCell ref="J58:Q58"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E003A556-D979-4BA4-9DE1-7709A1CBC03D}">
   <sheetPr>
@@ -3861,7 +3861,7 @@
   <dimension ref="A1:AW15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4779,7 +4779,7 @@
   <dimension ref="A1:AW15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,7 +5704,7 @@
   <dimension ref="A1:AS11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6460,7 +6460,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6481,7 +6481,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6496,7 +6496,7 @@
   <dimension ref="A2:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J44" sqref="J44:Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>